<commit_message>
AdBlock wrong path due to update - repair
* Correct path of AdBlock is detected correctly, bug is patched
* Some minor changes to variable naming and in-code documentation
</commit_message>
<xml_diff>
--- a/jobOffers.xlsx
+++ b/jobOffers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,1445 +453,969 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/power-platform-developer-architect-warszawa,oferta,1002040116?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-procurement-specialist-operations-warszawa,oferta,1002025032?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Power Platform Developer/ Architect</t>
+          <t>Senior Procurement Specialist (Operations)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Clouds On Mars sp. z o.o</t>
+          <t>AstraZeneca Pharma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/node-js-react-developer-masovian,oferta,9380789?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-social-media-warszawa,oferta,1002052708?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Node.js /React Developer</t>
+          <t>Specjalista ds. social media</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CRIF Sp. z o.o.</t>
+          <t>Grupa Mediowa Time</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-angular-mazowieckie,oferta,9354631?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/relocation-international-mobility-manager-masovian,oferta,9359482?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Front-End Developer (Angular)</t>
+          <t>Relocation - International Mobility Manager</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ASSECO DATA SYSTEMS S.A.</t>
+          <t>SOFTSWISS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-warszawa,oferta,1002022209?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/global-marketing-strategic-projects-expert-passenger-cars-warszawa,oferta,1002063515?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>.NET Developer</t>
+          <t>Global Marketing Strategic Projects Expert (Passenger Cars)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jeronimo Martins Polska S.A.</t>
+          <t>ZF Group</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/c-c%2b%2b-software-developer-in-iot-project-warszawa,oferta,1001989779?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/koordynator-ds-rozwoju-oferty-mazowieckie,oferta,9300424?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C/C++ Software developer in IoT Project</t>
+          <t>Koordynator ds. Rozwoju Oferty</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Integra Diagnostic – Projekt Sam się zbadaj</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-c%23-developer-warszawa,oferta,1002043726?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/product-manager-kardiologia-diabetologia-warszawa,oferta,1002055503?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Programista C# Developer</t>
+          <t>Product Manager – Kardiologia, Diabetologia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HARDWARE DIRECT</t>
+          <t>Aurovitas Pharma Polska sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/junior-php-js-developer-tech-support-warszawa,oferta,1002024864?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-warszawa,oferta,1002052537?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Junior PHP/JS Developer - Tech Support</t>
+          <t>Specjalista ds. Marketingu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RTB House</t>
+          <t>MAGMILLON SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/mid-full-stack-php-developer-mazowieckie,oferta,9329847?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-brand-manager-mlodszy-kierownik-ds-marki-warszawa,oferta,1002028533?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mid Full Stack PHP Developer</t>
+          <t>Junior Brand Manager / Młodszy Kierownik ds. Marki</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Grupa Kapitałowa VOX</t>
+          <t>Hortex Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-warszawa,oferta,1002049262?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/stazysta-tka-w-dziale-analiz-commercial-excellence-platny-staz-warszawa,oferta,1002031519?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Front-End Developer</t>
+          <t>Stażysta/tka w Dziale Analiz (Commercial Excellence) (Płatny staż)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>Sanofi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002049210?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-retail-planning-specialist-warszawa,oferta,1002072799?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>Senior Retail Planning Specialist</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-warszawa,oferta,1002049171?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/mechanical-design-engineer-comfort-warszawa,oferta,1002055242?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Java Developer</t>
+          <t>Mechanical Design Engineer Comfort</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>IKEA Purchasing Services Poland Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/backend-developer-warszawa,oferta,1002005373?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-media-planner-buyer-warszawa,oferta,1002008264?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Backend-Developer</t>
+          <t>Digital Media Planner/Buyer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TV Development GmbH</t>
+          <t>OMD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-net-%2b-angular-warszawa,oferta,1002043359?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/mlodszy-specjalista-ds-oskryptowania-w-badaniu-mediapanel-warszawa,oferta,1002028265?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fullstack Developer (.NET + Angular)</t>
+          <t>Młodszy Specjalista ds. Oskryptowania w Badaniu Mediapanel</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NATEK POLAND</t>
+          <t>Gemius SA</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-full-stack-software-engineer-risk-engineering-vice-president-warszawa,oferta,1002043309?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-trade-marketingu-warszawa,oferta,1002052143?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Senior Full-Stack Software Engineer - Risk Engineering - Vice President</t>
+          <t>Specjalista ds. Trade Marketingu</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Goldman Sachs Poland Services Sp. z o.o.</t>
+          <t>Herbapol Lublin S.A.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-with-react-angular-masovian,oferta,9367424?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/people-planner-digital-marketing-warszawa,oferta,1002028117?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>.NET Developer with React/ Angular</t>
+          <t>People Planner (digital marketing)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Objectivity sp. z o.o.</t>
+          <t>GroupM Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/development-manager-warszawa,oferta,1002021549?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/graphic-video-designer-warszawa,oferta,1002062711?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Development Manager</t>
+          <t>Graphic &amp; Video Designer</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Huuuge Games Sp. z o.o.</t>
+          <t>Sollers Consulting</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/node-js-developer-regular-warszawa,oferta,1002054948?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-warszawa,oferta,1002072191?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Node.js Developer (Regular)</t>
+          <t>Specjalista ds. Marketingu</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7N Sp. z o.o.</t>
+          <t>VILEA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-angular-%2b-java-warszawa,oferta,1002054928?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-marketing-communications-specialist-masovian,oferta,9339735?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fullstack Developer (Angular + Java)</t>
+          <t>Senior Marketing &amp; Communications Specialist</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7N Sp. z o.o.</t>
+          <t>PwC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-warszawa,oferta,1002043052?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/fundraise-r-ka-warszawa,oferta,1002048408?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Fundraise/r/ka</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Pentacomp</t>
+          <t>Fundacja Greenpeace Polska</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-rozwoj-platformy-dla-klienta-biznesowego-mazowieckie,oferta,9325618?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-analyst-warszawa,oferta,1002075274?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Java Developer - rozwój platformy dla klienta biznesowego</t>
+          <t>Marketing Analyst</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ING Bank Śląski S.A.</t>
+          <t>Avon Cosmetics Polska Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-wsparcie-procesow-kredytowych-mazowieckie,oferta,9325586?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/performance-specialist-warszawa,oferta,1002040060?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Java Developer – Wsparcie Procesów Kredytowych</t>
+          <t>Performance Specialist</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ING Bank Śląski S.A.</t>
+          <t>WebTalk Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/inzynier-devops-warszawa,oferta,1002065660?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-activation-specialist-warszawa,oferta,1002030648?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Inżynier DevOps</t>
+          <t>Marketing Activation Specialist</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Santander Bank Polska</t>
+          <t>British American Tobacco</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/mlodszy-analityk-programista-mlodszy-konsultant-it-warszawa,oferta,1002065637?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/performance-media-specialist-cee-warszawa,oferta,1002027276?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Młodszy Analityk Programista (Młodszy Konsultant IT)</t>
+          <t>Performance Media Specialist (CEE)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Accenture Consulting &amp; Strategy</t>
+          <t>PHD Media Direction Sp. Z o.o.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-digital-analyst-warszawa,oferta,1002023228?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/life-sciences-research-associate-manager-masovian,oferta,9331830?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Senior Digital Analyst</t>
+          <t>Life Sciences Research Associate Manager</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NetArch</t>
+          <t>Accenture Corporate Function</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/junior-node-js-developer-with-react-masovian,oferta,9360327?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/junior-marketing-manager-partnership-programme-warszawa,oferta,1002030640?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Junior Node.js Developer with React</t>
+          <t>Junior Marketing Manager (Partnership Programme)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-net-warszawa,oferta,1002054662?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-sales-representative-with-german-relocation-to-krakow-masovian,oferta,9352190?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Programista .NET</t>
+          <t>Digital Sales Representative with German (relocation to Kraków)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LUX MED Sp. z o.o.</t>
+          <t>TTEC EUROPE B.V. SP. Z O.O. ODDZIAŁ W POLSCE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002033363?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/it-researcher-warszawa,oferta,1002041894?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>IT Researcher</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Elmark Automatyka S.A.</t>
+          <t>NATEK POLAND</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/angular-frontend-developer-in-research-and-development-center-warszawa,oferta,1002065488?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/presentation-specialist-mon-fri-14-00-22-00-shift-warszawa,oferta,1002041756?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Angular Frontend Developer in Research and Development Center</t>
+          <t>Presentation Specialist Mon-Fri 14:00-22:00 shift</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>J.P. Morgan Poland Services sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-warszawa,oferta,1002065380?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-product-manager-produkcja-roslinna-mazowieckie,oferta,9363228?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Junior Product Manager - produkcja roślinna</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>PKO Bank Polski SA</t>
+          <t>PUH „Chemirol” sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-warszawa,oferta,1002065281?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/koordynator-ds-trade-marketingu-warszawa,oferta,1002058079?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Front-End Developer</t>
+          <t>Koordynator ds. Trade Marketingu</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>KAZAR Group Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-%D0%A1%D1%82%D0%B0%D1%80%D1%88%D0%B8%D0%B9-front-end-warszawa,oferta,1002065280?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/director-digital-operations-warszawa,oferta,1002065158?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Senior Front-End Developer / Старший Front-End розробник</t>
+          <t>Director, Digital Operations</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>Moderna Poland</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programistka-programista-programmer-warszawa,oferta,1002065279?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-account-executive-warszawa,oferta,1002050802?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Programistka / Programista / Programmer / Програміст</t>
+          <t>Junior Account Executive</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>Havas Engage Warsaw</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-developer-mazowieckie,oferta,9325337?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/personalized-internet-ads-assessor-masovian,oferta,9366169?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Personalized Internet Ads Assessor</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LUKANOVA CONSTRUCTION sp. z o.o.</t>
+          <t>Telus</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-and-hcl-domino-developer-warszawa,oferta,1002028676?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/customer-trade-marketing-manager-f-m-x-warszawa,oferta,1002053997?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Web and HCL Domino Developer</t>
+          <t>Customer/Trade Marketing Manager (f/m/x)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"PEDERSEN&amp;PARTNERS" sp. z o.o.</t>
+          <t>Mars Polska sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/angular-frontend-developer-warszawa,oferta,1001967179?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/commercial-lead-poland-masovian,oferta,9351506?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Angular Frontend Developer</t>
+          <t>Commercial Lead - Poland</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Gigaset Communications Polska</t>
+          <t>Wyser Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-ruby-on-rails-developer-warszawa,oferta,1002014117?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/pos-application-specialist-terminal-integration-engineer-warszawa,oferta,1002054021?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Senior Ruby on Rails Developer</t>
+          <t>POS Application Specialist (Terminal Integration Engineer)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>codequest sp. z o.o.</t>
+          <t>Worldline Financial Services (Europe) S.A. Spółka Akcyjna</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-with-java-and-kotlin-warszawa,oferta,1001988263?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/junior-marketing-manager-warszawa,oferta,1002030392?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fullstack Developer with Java and Kotlin</t>
+          <t>Junior Marketing Manager</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Flotman Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-in-samsung-pay-project-warszawa,oferta,1001998322?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/market-research-senior-specialist-warszawa,oferta,1002023380?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Java Developer in Samsung Pay Project</t>
+          <t>Market Research Senior Specialist</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Wavemaker Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-angular-warszawa,oferta,1002042645?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-online-marketing-specialist-with-romanian-warszawa,oferta,1002040766?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Senior Front-end Developer (Angular)</t>
+          <t>Junior Online Marketing specialist with Romanian</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Goldman Recruitment</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-react-warszawa,oferta,1002042169?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/model-risk-management-associate-warszawa,oferta,1002023073?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Senior Front-end Developer (React)</t>
+          <t>Model Risk Management | Associate</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Goldman Sachs Poland Services Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-security-engineer-warszawa,oferta,1002042581?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-ads-specialist-with-romanian-warszawa,oferta,1002040743?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Senior Security Engineer</t>
+          <t>Marketing &amp; Ads Specialist with Romanian</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Arche Consulting Sp z o.o.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/internship-intern-in-language-data-operations-group-warszawa,oferta,1002042311?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/menadzer-produktu-oze-pompy-ciepla-rekuperacja-mazowieckie,oferta,9362352?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Internship - Intern in Language Data Operations Group</t>
+          <t>Menadżer Produktu OZE – pompy ciepła, rekuperacja</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>TWEETOP Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-masovian,oferta,9366382?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/d2c-performance-senior-specialist-warszawa,oferta,1002053458?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>D2C Performance Senior Specialist</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktyki-php-magento-mazowieckie,oferta,9366562?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/e-commerce-specialist-warszawa,oferta,1002053407?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Praktyki PHP/ Magento</t>
+          <t>E-commerce Specialist</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Accenture Technology</t>
+          <t>Verestro S.A.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-mazowieckie,oferta,9342249?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/video-host-community-manager-mazowieckie,oferta,9331323?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Frontend Developer</t>
+          <t>Video host / Community Manager</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Simplicity Recruitment</t>
+          <t>Woodpecker.co</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/python-developer-mazowieckie,oferta,9366075?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-los-pow-piaseczynski,oferta,1002061107?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Python Developer</t>
+          <t>Specjalista ds. marketingu</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>EOS Poland Sp. z o.o.</t>
+          <t>SCANDINAVIAN BABY PIOTR DMOWSKI SPÓŁKA KOMANDYTOWA</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-net-%2b-angular-warszawa,oferta,1002053849?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/content-editor-m-f-d-warszawa,oferta,1002061096?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fullstack Developer (.NET + Angular)</t>
+          <t>Content Editor (m/f/d)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Westwing.pl</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-publisher-warszawa,oferta,1002032982?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/account-manager-warszawa,oferta,1002056335?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Web Publisher</t>
+          <t>Account Manager</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CHEIL POLAND</t>
+          <t>Sales &amp; More SA</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktykant-w-zespole-automatyzacji-testow-warszawa,oferta,1002053843?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/squad-group-lead-it-delivery-manager-masovian,oferta,9350392?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Praktykant w zespole automatyzacji testów</t>
+          <t>Squad Group Lead/ IT Delivery Manager</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Nokia</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-z-vue-js-warszawa,oferta,1002053844?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/brand-manager-health-medical-solutions-warszawa,oferta,1002029234?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Frontend Developer z Vue.js</t>
+          <t>Brand Manager (Health &amp; Medical Solutions)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Essity Poland Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktykant-w-zespole-programistow-warszawa,oferta,1002053832?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-ppc-specialist-warszawa,oferta,1002070471?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Praktykant w zespole programistów</t>
+          <t>Senior PPC Specialist</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Pracuj.pl dla Firm</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-architect-warszawa,oferta,1002001855?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/operations-process-analyst-masovian,oferta,9338219?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Frontend Architect</t>
+          <t>Operations Process Analyst</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Grupa Pracuj</t>
+          <t>GetResponse</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/elasticsearch-developer-warszawa,oferta,1002047999?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/product-manager-regulatory-risk-warszawa,oferta,1002049794?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ElasticSearch Developer</t>
+          <t>Product Manager - Regulatory Risk</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ASTEK Polska</t>
+          <t>TransferGo</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/specjalista-seo-mazowieckie,oferta,9378711?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/logistics-staff-warszawa,oferta,1002049666?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Specjalista SEO</t>
+          <t>Logistics Staff</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Grupa Tense Polska spółka z ograniczoną odpowiedzialnością spółka komandytowa</t>
+          <t>SAMSUNG SDS GLOBAL SCL POLAND Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-warszawa,oferta,1002017663?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/social-media-buyer-warszawa,oferta,1002028975?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>.NET developer</t>
+          <t>Social Media Buyer</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ITCenter Sp. z o.o. Sp. k.</t>
+          <t>Wyborowa Pernod Ricard</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-backend-software-engineer-mazowieckie,oferta,9356066?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-communication-manager-warszawa,oferta,1002049606?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Senior Backend Software Engineer</t>
+          <t>Digital Communication Manager</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>DOBRYMECHANIK.PL SPOŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Michael Page</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-mazowieckie,oferta,9331303?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/paid-media-specialist-warszawa,oferta,1002055767?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Paid Media Specialist</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>3e Software House</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/business-intelligence-junior-and-mid-level-developer-in-risk-warszawa,oferta,1002064807?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Business Intelligence Junior and Mid level Developer in Risk</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Citi Poland</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/asp-net-developer-mazowieckie,oferta,9331273?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>ASP.NET Developer</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Simplicity Recruitment</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-iot-warszawa,oferta,1002006753?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Fullstack Developer (IOT)</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Reply Polska Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/programistka-programista-net-warszawa,oferta,1002047806?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Programistka / Programista .NET</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Benefit Systems S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/javascript-test-developer-e-commerce-warszawa,oferta,1002064673?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>JavaScript Test Developer – e-commerce</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>SII Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/programista-programistka-react-native-warszawa,oferta,1002057171?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Programista/Programistka React Native</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Benefit Systems S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-net-developer-masovian,oferta,9369671?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Senior .NET Developer</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/test-automation-engineer-mazowieckie,oferta,9365617?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Test Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Craftware Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/digital-analyst-analityczka-analityk-digital-warszawa,oferta,1002064518?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Digital Analyst - Analityczka/Analityk Digital</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>UNIQA</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-angular-developer-masovian,oferta,9369633?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Senior Angular Developer</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-react-developer-masovian,oferta,9369594?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Senior React Developer</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-qa-automation-engineer-warszawa,oferta,1002050234?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Senior QA Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>ITECHART GROUP sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/middle-qa-automation-engineer-warszawa,oferta,1002050232?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Middle QA Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>ITECHART GROUP sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-automatyzujacy-warszawa,oferta,1002053411?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Tester automatyzujący</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>7N Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002020133?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Full Stack Developer</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>POLSKA PRESS SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-oprogramowania-warszawa,oferta,1002020113?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Tester oprogramowania</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Centralny Ośrodek Informatyki</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/react-developer-warszawa,oferta,1002064311?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>React Developer</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>9bits Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/fullstack-net-developer-warszawa,oferta,1002064222?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Fullstack .NET Developer</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>eService Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/specjalista-ds-seo-mazowieckie,oferta,9341539?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Specjalista ds. SEO</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Sunrise System sp. z o.o. sp. k.</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/back-end-developer-warszawa,oferta,1002019932?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Back-end Developer</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>POLSKA PRESS SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/cms-backend-developer-mazowieckie,oferta,9327135?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>CMS Backend Developer</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Josera Polska</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-warszawa,oferta,1002032262?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Frontend Developer</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>JT Weston sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/software-developer-java-spring-hibernate-warszawa,oferta,1002063962?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Software Developer (Java, Spring/Hibernate)</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>ALIOR BANK</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/specjalista-ds-rozwoju-oprogramowania-warszawa,oferta,1002063926?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Specjalista ds. Rozwoju Oprogramowania</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>ALIOR BANK</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/junior-frontend-developer-mazowieckie,oferta,9377584?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Junior Frontend Developer</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>DOBRYMECHANIK.PL SPOŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/java-developer-masovian,oferta,9358512?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Java Developer</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>ING Bank Śląski S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/konsultant-bi-warszawa,oferta,1002019667?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Konsultant BI</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Cogit sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-ze-znajomoscia-sql-mozliwosc-rozwoju-w-kierunku-automatyzacji-mazowieckie,oferta,9377481?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Tester ze znajomością SQL - możliwość rozwoju w kierunku automatyzacji</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>BEST S.A.</t>
+          <t>Sales &amp; More SA</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
AdBlock wrong path due to update - repair (#8)
* Correct path of AdBlock is detected correctly, bug is patched
* Some minor changes to variable naming and in-code documentation
</commit_message>
<xml_diff>
--- a/jobOffers.xlsx
+++ b/jobOffers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,1445 +453,969 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/power-platform-developer-architect-warszawa,oferta,1002040116?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-procurement-specialist-operations-warszawa,oferta,1002025032?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Power Platform Developer/ Architect</t>
+          <t>Senior Procurement Specialist (Operations)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Clouds On Mars sp. z o.o</t>
+          <t>AstraZeneca Pharma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/node-js-react-developer-masovian,oferta,9380789?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-social-media-warszawa,oferta,1002052708?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Node.js /React Developer</t>
+          <t>Specjalista ds. social media</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CRIF Sp. z o.o.</t>
+          <t>Grupa Mediowa Time</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-angular-mazowieckie,oferta,9354631?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/relocation-international-mobility-manager-masovian,oferta,9359482?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Front-End Developer (Angular)</t>
+          <t>Relocation - International Mobility Manager</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ASSECO DATA SYSTEMS S.A.</t>
+          <t>SOFTSWISS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-warszawa,oferta,1002022209?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/global-marketing-strategic-projects-expert-passenger-cars-warszawa,oferta,1002063515?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>.NET Developer</t>
+          <t>Global Marketing Strategic Projects Expert (Passenger Cars)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Jeronimo Martins Polska S.A.</t>
+          <t>ZF Group</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/c-c%2b%2b-software-developer-in-iot-project-warszawa,oferta,1001989779?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/koordynator-ds-rozwoju-oferty-mazowieckie,oferta,9300424?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C/C++ Software developer in IoT Project</t>
+          <t>Koordynator ds. Rozwoju Oferty</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Integra Diagnostic – Projekt Sam się zbadaj</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-c%23-developer-warszawa,oferta,1002043726?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/product-manager-kardiologia-diabetologia-warszawa,oferta,1002055503?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Programista C# Developer</t>
+          <t>Product Manager – Kardiologia, Diabetologia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HARDWARE DIRECT</t>
+          <t>Aurovitas Pharma Polska sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/junior-php-js-developer-tech-support-warszawa,oferta,1002024864?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-warszawa,oferta,1002052537?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Junior PHP/JS Developer - Tech Support</t>
+          <t>Specjalista ds. Marketingu</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RTB House</t>
+          <t>MAGMILLON SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/mid-full-stack-php-developer-mazowieckie,oferta,9329847?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-brand-manager-mlodszy-kierownik-ds-marki-warszawa,oferta,1002028533?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mid Full Stack PHP Developer</t>
+          <t>Junior Brand Manager / Młodszy Kierownik ds. Marki</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Grupa Kapitałowa VOX</t>
+          <t>Hortex Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-warszawa,oferta,1002049262?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/stazysta-tka-w-dziale-analiz-commercial-excellence-platny-staz-warszawa,oferta,1002031519?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Front-End Developer</t>
+          <t>Stażysta/tka w Dziale Analiz (Commercial Excellence) (Płatny staż)</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>Sanofi</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002049210?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-retail-planning-specialist-warszawa,oferta,1002072799?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>Senior Retail Planning Specialist</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-warszawa,oferta,1002049171?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/mechanical-design-engineer-comfort-warszawa,oferta,1002055242?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Java Developer</t>
+          <t>Mechanical Design Engineer Comfort</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Robert Bosch Sp. z o.o.</t>
+          <t>IKEA Purchasing Services Poland Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/backend-developer-warszawa,oferta,1002005373?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-media-planner-buyer-warszawa,oferta,1002008264?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Backend-Developer</t>
+          <t>Digital Media Planner/Buyer</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>TV Development GmbH</t>
+          <t>OMD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-net-%2b-angular-warszawa,oferta,1002043359?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/mlodszy-specjalista-ds-oskryptowania-w-badaniu-mediapanel-warszawa,oferta,1002028265?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fullstack Developer (.NET + Angular)</t>
+          <t>Młodszy Specjalista ds. Oskryptowania w Badaniu Mediapanel</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NATEK POLAND</t>
+          <t>Gemius SA</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-full-stack-software-engineer-risk-engineering-vice-president-warszawa,oferta,1002043309?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-trade-marketingu-warszawa,oferta,1002052143?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Senior Full-Stack Software Engineer - Risk Engineering - Vice President</t>
+          <t>Specjalista ds. Trade Marketingu</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Goldman Sachs Poland Services Sp. z o.o.</t>
+          <t>Herbapol Lublin S.A.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-with-react-angular-masovian,oferta,9367424?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/people-planner-digital-marketing-warszawa,oferta,1002028117?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>.NET Developer with React/ Angular</t>
+          <t>People Planner (digital marketing)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Objectivity sp. z o.o.</t>
+          <t>GroupM Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/development-manager-warszawa,oferta,1002021549?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/graphic-video-designer-warszawa,oferta,1002062711?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Development Manager</t>
+          <t>Graphic &amp; Video Designer</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Huuuge Games Sp. z o.o.</t>
+          <t>Sollers Consulting</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/node-js-developer-regular-warszawa,oferta,1002054948?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-warszawa,oferta,1002072191?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Node.js Developer (Regular)</t>
+          <t>Specjalista ds. Marketingu</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7N Sp. z o.o.</t>
+          <t>VILEA SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-angular-%2b-java-warszawa,oferta,1002054928?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-marketing-communications-specialist-masovian,oferta,9339735?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fullstack Developer (Angular + Java)</t>
+          <t>Senior Marketing &amp; Communications Specialist</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7N Sp. z o.o.</t>
+          <t>PwC</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-warszawa,oferta,1002043052?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/fundraise-r-ka-warszawa,oferta,1002048408?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Fundraise/r/ka</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Pentacomp</t>
+          <t>Fundacja Greenpeace Polska</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-rozwoj-platformy-dla-klienta-biznesowego-mazowieckie,oferta,9325618?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-analyst-warszawa,oferta,1002075274?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Java Developer - rozwój platformy dla klienta biznesowego</t>
+          <t>Marketing Analyst</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ING Bank Śląski S.A.</t>
+          <t>Avon Cosmetics Polska Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-wsparcie-procesow-kredytowych-mazowieckie,oferta,9325586?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/performance-specialist-warszawa,oferta,1002040060?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Java Developer – Wsparcie Procesów Kredytowych</t>
+          <t>Performance Specialist</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ING Bank Śląski S.A.</t>
+          <t>WebTalk Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/inzynier-devops-warszawa,oferta,1002065660?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-activation-specialist-warszawa,oferta,1002030648?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Inżynier DevOps</t>
+          <t>Marketing Activation Specialist</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Santander Bank Polska</t>
+          <t>British American Tobacco</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/mlodszy-analityk-programista-mlodszy-konsultant-it-warszawa,oferta,1002065637?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/performance-media-specialist-cee-warszawa,oferta,1002027276?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Młodszy Analityk Programista (Młodszy Konsultant IT)</t>
+          <t>Performance Media Specialist (CEE)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Accenture Consulting &amp; Strategy</t>
+          <t>PHD Media Direction Sp. Z o.o.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-digital-analyst-warszawa,oferta,1002023228?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/life-sciences-research-associate-manager-masovian,oferta,9331830?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Senior Digital Analyst</t>
+          <t>Life Sciences Research Associate Manager</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>NetArch</t>
+          <t>Accenture Corporate Function</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/junior-node-js-developer-with-react-masovian,oferta,9360327?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/junior-marketing-manager-partnership-programme-warszawa,oferta,1002030640?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Junior Node.js Developer with React</t>
+          <t>Junior Marketing Manager (Partnership Programme)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-net-warszawa,oferta,1002054662?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-sales-representative-with-german-relocation-to-krakow-masovian,oferta,9352190?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Programista .NET</t>
+          <t>Digital Sales Representative with German (relocation to Kraków)</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LUX MED Sp. z o.o.</t>
+          <t>TTEC EUROPE B.V. SP. Z O.O. ODDZIAŁ W POLSCE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002033363?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/it-researcher-warszawa,oferta,1002041894?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>IT Researcher</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Elmark Automatyka S.A.</t>
+          <t>NATEK POLAND</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/angular-frontend-developer-in-research-and-development-center-warszawa,oferta,1002065488?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/presentation-specialist-mon-fri-14-00-22-00-shift-warszawa,oferta,1002041756?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Angular Frontend Developer in Research and Development Center</t>
+          <t>Presentation Specialist Mon-Fri 14:00-22:00 shift</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>J.P. Morgan Poland Services sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-warszawa,oferta,1002065380?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-product-manager-produkcja-roslinna-mazowieckie,oferta,9363228?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Junior Product Manager - produkcja roślinna</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>PKO Bank Polski SA</t>
+          <t>PUH „Chemirol” sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/front-end-developer-warszawa,oferta,1002065281?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/koordynator-ds-trade-marketingu-warszawa,oferta,1002058079?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Front-End Developer</t>
+          <t>Koordynator ds. Trade Marketingu</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>KAZAR Group Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-%D0%A1%D1%82%D0%B0%D1%80%D1%88%D0%B8%D0%B9-front-end-warszawa,oferta,1002065280?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/director-digital-operations-warszawa,oferta,1002065158?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Senior Front-End Developer / Старший Front-End розробник</t>
+          <t>Director, Digital Operations</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>Moderna Poland</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programistka-programista-programmer-warszawa,oferta,1002065279?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-account-executive-warszawa,oferta,1002050802?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Programistka / Programista / Programmer / Програміст</t>
+          <t>Junior Account Executive</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Uniwersytet Warszawski</t>
+          <t>Havas Engage Warsaw</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-developer-mazowieckie,oferta,9325337?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/personalized-internet-ads-assessor-masovian,oferta,9366169?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Personalized Internet Ads Assessor</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LUKANOVA CONSTRUCTION sp. z o.o.</t>
+          <t>Telus</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-and-hcl-domino-developer-warszawa,oferta,1002028676?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/customer-trade-marketing-manager-f-m-x-warszawa,oferta,1002053997?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Web and HCL Domino Developer</t>
+          <t>Customer/Trade Marketing Manager (f/m/x)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"PEDERSEN&amp;PARTNERS" sp. z o.o.</t>
+          <t>Mars Polska sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/angular-frontend-developer-warszawa,oferta,1001967179?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/commercial-lead-poland-masovian,oferta,9351506?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Angular Frontend Developer</t>
+          <t>Commercial Lead - Poland</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Gigaset Communications Polska</t>
+          <t>Wyser Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-ruby-on-rails-developer-warszawa,oferta,1002014117?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/pos-application-specialist-terminal-integration-engineer-warszawa,oferta,1002054021?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Senior Ruby on Rails Developer</t>
+          <t>POS Application Specialist (Terminal Integration Engineer)</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>codequest sp. z o.o.</t>
+          <t>Worldline Financial Services (Europe) S.A. Spółka Akcyjna</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-with-java-and-kotlin-warszawa,oferta,1001988263?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/junior-marketing-manager-warszawa,oferta,1002030392?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fullstack Developer with Java and Kotlin</t>
+          <t>Junior Marketing Manager</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Flotman Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/java-developer-in-samsung-pay-project-warszawa,oferta,1001998322?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/market-research-senior-specialist-warszawa,oferta,1002023380?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Java Developer in Samsung Pay Project</t>
+          <t>Market Research Senior Specialist</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>Wavemaker Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-angular-warszawa,oferta,1002042645?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/junior-online-marketing-specialist-with-romanian-warszawa,oferta,1002040766?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Senior Front-end Developer (Angular)</t>
+          <t>Junior Online Marketing specialist with Romanian</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Goldman Recruitment</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-front-end-developer-react-warszawa,oferta,1002042169?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/model-risk-management-associate-warszawa,oferta,1002023073?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Senior Front-end Developer (React)</t>
+          <t>Model Risk Management | Associate</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Goldman Sachs Poland Services Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-security-engineer-warszawa,oferta,1002042581?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/marketing-ads-specialist-with-romanian-warszawa,oferta,1002040743?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Senior Security Engineer</t>
+          <t>Marketing &amp; Ads Specialist with Romanian</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Future Processing S.A.</t>
+          <t>Arche Consulting Sp z o.o.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/internship-intern-in-language-data-operations-group-warszawa,oferta,1002042311?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/menadzer-produktu-oze-pompy-ciepla-rekuperacja-mazowieckie,oferta,9362352?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Internship - Intern in Language Data Operations Group</t>
+          <t>Menadżer Produktu OZE – pompy ciepła, rekuperacja</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Samsung R&amp;D Institute Poland</t>
+          <t>TWEETOP Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-masovian,oferta,9366382?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/d2c-performance-senior-specialist-warszawa,oferta,1002053458?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>D2C Performance Senior Specialist</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Nokia</t>
+          <t>Samsung Electronics Polska</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktyki-php-magento-mazowieckie,oferta,9366562?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/e-commerce-specialist-warszawa,oferta,1002053407?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Praktyki PHP/ Magento</t>
+          <t>E-commerce Specialist</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Accenture Technology</t>
+          <t>Verestro S.A.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-mazowieckie,oferta,9342249?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/video-host-community-manager-mazowieckie,oferta,9331323?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Frontend Developer</t>
+          <t>Video host / Community Manager</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Simplicity Recruitment</t>
+          <t>Woodpecker.co</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/python-developer-mazowieckie,oferta,9366075?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/specjalista-ds-marketingu-los-pow-piaseczynski,oferta,1002061107?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Python Developer</t>
+          <t>Specjalista ds. marketingu</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>EOS Poland Sp. z o.o.</t>
+          <t>SCANDINAVIAN BABY PIOTR DMOWSKI SPÓŁKA KOMANDYTOWA</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-net-%2b-angular-warszawa,oferta,1002053849?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/content-editor-m-f-d-warszawa,oferta,1002061096?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Fullstack Developer (.NET + Angular)</t>
+          <t>Content Editor (m/f/d)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Westwing.pl</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/web-publisher-warszawa,oferta,1002032982?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/account-manager-warszawa,oferta,1002056335?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Web Publisher</t>
+          <t>Account Manager</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CHEIL POLAND</t>
+          <t>Sales &amp; More SA</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktykant-w-zespole-automatyzacji-testow-warszawa,oferta,1002053843?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/squad-group-lead-it-delivery-manager-masovian,oferta,9350392?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Praktykant w zespole automatyzacji testów</t>
+          <t>Squad Group Lead/ IT Delivery Manager</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Nokia</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-z-vue-js-warszawa,oferta,1002053844?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/brand-manager-health-medical-solutions-warszawa,oferta,1002029234?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Frontend Developer z Vue.js</t>
+          <t>Brand Manager (Health &amp; Medical Solutions)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Essity Poland Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/praktykant-w-zespole-programistow-warszawa,oferta,1002053832?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/senior-ppc-specialist-warszawa,oferta,1002070471?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Praktykant w zespole programistów</t>
+          <t>Senior PPC Specialist</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>AXA Avanssur SA Oddział II w Polsce</t>
+          <t>Pracuj.pl dla Firm</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/frontend-architect-warszawa,oferta,1002001855?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
+          <t>https://www.pracuj.pl/praca/operations-process-analyst-masovian,oferta,9338219?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Frontend Architect</t>
+          <t>Operations Process Analyst</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Grupa Pracuj</t>
+          <t>GetResponse</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/elasticsearch-developer-warszawa,oferta,1002047999?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/product-manager-regulatory-risk-warszawa,oferta,1002049794?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ElasticSearch Developer</t>
+          <t>Product Manager - Regulatory Risk</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ASTEK Polska</t>
+          <t>TransferGo</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/specjalista-seo-mazowieckie,oferta,9378711?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/logistics-staff-warszawa,oferta,1002049666?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Specjalista SEO</t>
+          <t>Logistics Staff</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Grupa Tense Polska spółka z ograniczoną odpowiedzialnością spółka komandytowa</t>
+          <t>SAMSUNG SDS GLOBAL SCL POLAND Sp. z o.o.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/net-developer-warszawa,oferta,1002017663?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/social-media-buyer-warszawa,oferta,1002028975?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>.NET developer</t>
+          <t>Social Media Buyer</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ITCenter Sp. z o.o. Sp. k.</t>
+          <t>Wyborowa Pernod Ricard</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/senior-backend-software-engineer-mazowieckie,oferta,9356066?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/digital-communication-manager-warszawa,oferta,1002049606?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Senior Backend Software Engineer</t>
+          <t>Digital Communication Manager</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>DOBRYMECHANIK.PL SPOŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
+          <t>Michael Page</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>https://www.pracuj.pl/praca/programista-java-mazowieckie,oferta,9331303?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
+          <t>https://www.pracuj.pl/praca/paid-media-specialist-warszawa,oferta,1002055767?s=6488642a&amp;searchId=e00cdcc0-31be-11ed-b9f8-c1a8d935d73e</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Programista Java</t>
+          <t>Paid Media Specialist</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>3e Software House</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/business-intelligence-junior-and-mid-level-developer-in-risk-warszawa,oferta,1002064807?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Business Intelligence Junior and Mid level Developer in Risk</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Citi Poland</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/asp-net-developer-mazowieckie,oferta,9331273?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>ASP.NET Developer</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Simplicity Recruitment</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/fullstack-developer-iot-warszawa,oferta,1002006753?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Fullstack Developer (IOT)</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Reply Polska Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/programistka-programista-net-warszawa,oferta,1002047806?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Programistka / Programista .NET</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Benefit Systems S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/javascript-test-developer-e-commerce-warszawa,oferta,1002064673?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>JavaScript Test Developer – e-commerce</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>SII Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/programista-programistka-react-native-warszawa,oferta,1002057171?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Programista/Programistka React Native</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Benefit Systems S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-net-developer-masovian,oferta,9369671?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Senior .NET Developer</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/test-automation-engineer-mazowieckie,oferta,9365617?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Test Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Craftware Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/digital-analyst-analityczka-analityk-digital-warszawa,oferta,1002064518?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Digital Analyst - Analityczka/Analityk Digital</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>UNIQA</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-angular-developer-masovian,oferta,9369633?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Senior Angular Developer</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-react-developer-masovian,oferta,9369594?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Senior React Developer</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>QODECA sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/senior-qa-automation-engineer-warszawa,oferta,1002050234?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Senior QA Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>ITECHART GROUP sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/middle-qa-automation-engineer-warszawa,oferta,1002050232?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d&amp;rel=rwd&amp;rel=rwd</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Middle QA Automation Engineer</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>ITECHART GROUP sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-automatyzujacy-warszawa,oferta,1002053411?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Tester automatyzujący</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>7N Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/full-stack-developer-warszawa,oferta,1002020133?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Full Stack Developer</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>POLSKA PRESS SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-oprogramowania-warszawa,oferta,1002020113?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Tester oprogramowania</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Centralny Ośrodek Informatyki</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/react-developer-warszawa,oferta,1002064311?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>React Developer</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>9bits Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/fullstack-net-developer-warszawa,oferta,1002064222?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Fullstack .NET Developer</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>eService Sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/specjalista-ds-seo-mazowieckie,oferta,9341539?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Specjalista ds. SEO</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Sunrise System sp. z o.o. sp. k.</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/back-end-developer-warszawa,oferta,1002019932?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Back-end Developer</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>POLSKA PRESS SPÓŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/cms-backend-developer-mazowieckie,oferta,9327135?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>CMS Backend Developer</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Josera Polska</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/frontend-developer-warszawa,oferta,1002032262?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Frontend Developer</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>JT Weston sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/software-developer-java-spring-hibernate-warszawa,oferta,1002063962?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Software Developer (Java, Spring/Hibernate)</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>ALIOR BANK</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/specjalista-ds-rozwoju-oprogramowania-warszawa,oferta,1002063926?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Specjalista ds. Rozwoju Oprogramowania</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>ALIOR BANK</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/junior-frontend-developer-mazowieckie,oferta,9377584?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Junior Frontend Developer</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>DOBRYMECHANIK.PL SPOŁKA Z OGRANICZONĄ ODPOWIEDZIALNOŚCIĄ</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/java-developer-masovian,oferta,9358512?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Java Developer</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>ING Bank Śląski S.A.</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/konsultant-bi-warszawa,oferta,1002019667?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Konsultant BI</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Cogit sp. z o.o.</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>https://www.pracuj.pl/praca/tester-ze-znajomoscia-sql-mozliwosc-rozwoju-w-kierunku-automatyzacji-mazowieckie,oferta,9377481?s=ecf34d40&amp;searchId=2cb579e0-2e9c-11ed-b5ae-6f0d2088881d</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Tester ze znajomością SQL - możliwość rozwoju w kierunku automatyzacji</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>BEST S.A.</t>
+          <t>Sales &amp; More SA</t>
         </is>
       </c>
     </row>

</xml_diff>